<commit_message>
Mise à jour 0.1.1 - LET'S FIGHT!
Écran de combat
-Tous les boutons sont mis en place
-Tous les champs sont nommés et présents
-Linking entre les boutons du menu principal pour se rendre au combat
fait
-Le bouton fuir est une image (encore à améliorer) et fonctionne (ramène
au menu principal)

Correctifs divers
-Correctif des margins dans l'écran de choix de personnage
-Refactorisation de tous les noms d'écrans pour qu'ils aient "Ecran"
exemple : "EcranMenuPrincipal"
-Modification des MessageBox d'erreur lors de la connexion pour qu'ils
soient plus propres et professionnels
</commit_message>
<xml_diff>
--- a/Audits/sommaireAudit2.xlsx
+++ b/Audits/sommaireAudit2.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wthemens\Combaxe\Audits\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>No tâche</t>
   </si>
@@ -162,6 +157,12 @@
   </si>
   <si>
     <t>Trouver et assigner des images aux personnages et ennemis</t>
+  </si>
+  <si>
+    <t>Tom a fini 23 Oct 2014 / Demande lui ses heures</t>
+  </si>
+  <si>
+    <t>Commencé par Antho 23 Oct 2014 - 21:30</t>
   </si>
 </sst>
 </file>
@@ -227,7 +228,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -384,7 +405,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -419,7 +440,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -596,7 +617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -604,21 +625,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54.5703125" customWidth="1"/>
     <col min="3" max="3" width="51.42578125" customWidth="1"/>
     <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,7 +660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>19</v>
       </c>
@@ -656,7 +678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>20</v>
       </c>
@@ -674,7 +696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>21</v>
       </c>
@@ -692,7 +714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>22</v>
       </c>
@@ -709,8 +731,11 @@
       <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -728,7 +753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>14</v>
       </c>
@@ -747,8 +772,11 @@
       <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>16</v>
       </c>
@@ -768,7 +796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>23</v>
       </c>
@@ -788,7 +816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>24</v>
       </c>
@@ -808,7 +836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>13</v>
       </c>
@@ -828,7 +856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>25</v>
       </c>
@@ -848,7 +876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>26</v>
       </c>
@@ -868,7 +896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>27</v>
       </c>
@@ -888,7 +916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>28</v>
       </c>
@@ -908,7 +936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>29</v>
       </c>
@@ -1061,44 +1089,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2 A3:F19">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Terminé">
+  <conditionalFormatting sqref="F2 A3:F19 G7 G5">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D4)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Mise à jour Audit pour mes tâches
</commit_message>
<xml_diff>
--- a/Audits/sommaireAudit2.xlsx
+++ b/Audits/sommaireAudit2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>No tâche</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>Tom a fini 23 Oct 2014 / Demande lui ses heures</t>
-  </si>
-  <si>
-    <t>Commencé par Antho 23 Oct 2014 - 21:30</t>
   </si>
 </sst>
 </file>
@@ -228,27 +225,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -627,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,14 +703,12 @@
         <v>14</v>
       </c>
       <c r="E5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -770,7 +745,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>46</v>
@@ -1043,7 +1018,7 @@
       </c>
       <c r="E21" s="2">
         <f t="array" ref="E21">SUM(E2:E20)</f>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -1089,44 +1064,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2 A3:F19 G7 G5">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D4)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Mise à jour 0.1.2 - Linking boutons Menu principal
</commit_message>
<xml_diff>
--- a/Audits/sommaireAudit2.xlsx
+++ b/Audits/sommaireAudit2.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Combaxe\Combaxe\Audits\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -594,7 +599,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -604,11 +609,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54.5703125" customWidth="1"/>
     <col min="3" max="3" width="51.42578125" customWidth="1"/>

</xml_diff>

<commit_message>
début et fini de parser les donnees du joueur
j'ai mit les donnees d'un personnage dans un combat
modification
personnage.cs
csproj
ecrancombat
</commit_message>
<xml_diff>
--- a/Audits/sommaireAudit2.xlsx
+++ b/Audits/sommaireAudit2.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Combaxe\Combaxe\Audits\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>No tâche</t>
   </si>
@@ -165,6 +160,9 @@
   </si>
   <si>
     <t>Tom a fini 23 Oct 2014 / Demande lui ses heures</t>
+  </si>
+  <si>
+    <t>fini … un peu random comme image mais fonctionnelle, le temps est GOOD</t>
   </si>
 </sst>
 </file>
@@ -230,7 +228,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -599,7 +607,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -610,7 +618,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,10 +838,13 @@
         <v>15</v>
       </c>
       <c r="E11" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1023,7 +1034,7 @@
       </c>
       <c r="E21" s="2">
         <f t="array" ref="E21">SUM(E2:E20)</f>
-        <v>69</v>
+        <v>67.5</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -1069,44 +1080,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2 A3:F19 G7 G5">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Terminé">
+  <conditionalFormatting sqref="F2 A3:F19 G7 G5 G11">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D4)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Mise à jour 0.1.3a
*Ajout des champs profession et niveau dans l'écran
"EcranInventaireMagasin"
*Mise à jour de l'audit concernant mes tâches
</commit_message>
<xml_diff>
--- a/Audits/sommaireAudit2.xlsx
+++ b/Audits/sommaireAudit2.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Combaxe\Combaxe\Audits\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -599,7 +594,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -610,10 +605,10 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54.5703125" customWidth="1"/>
     <col min="3" max="3" width="51.42578125" customWidth="1"/>
@@ -672,10 +667,10 @@
         <v>14</v>
       </c>
       <c r="E3" s="2">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -690,10 +685,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -853,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1023,7 +1018,7 @@
       </c>
       <c r="E21" s="2">
         <f t="array" ref="E21">SUM(E2:E20)</f>
-        <v>69</v>
+        <v>65.5</v>
       </c>
       <c r="F21" s="2"/>
     </row>

</xml_diff>